<commit_message>
Corrigindo conteúdo de gráficos.
</commit_message>
<xml_diff>
--- a/Testes/Threadring/Threadring - 10000 process.xlsx
+++ b/Testes/Threadring/Threadring - 10000 process.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="11">
   <si>
     <t>Erlang</t>
   </si>
@@ -39,12 +39,6 @@
   </si>
   <si>
     <t>Scala - Normal</t>
-  </si>
-  <si>
-    <t>Tempo médio</t>
-  </si>
-  <si>
-    <t>Tempo total</t>
   </si>
   <si>
     <t>Scala-Default</t>
@@ -583,11 +577,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="83753984"/>
-        <c:axId val="76880640"/>
+        <c:axId val="97438208"/>
+        <c:axId val="67376768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83753984"/>
+        <c:axId val="97438208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -607,7 +601,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76880640"/>
+        <c:crossAx val="67376768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -615,7 +609,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76880640"/>
+        <c:axId val="67376768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -645,7 +639,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83753984"/>
+        <c:crossAx val="97438208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1108,11 +1102,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96385536"/>
-        <c:axId val="60417152"/>
+        <c:axId val="122310656"/>
+        <c:axId val="122052608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96385536"/>
+        <c:axId val="122310656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1132,7 +1126,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60417152"/>
+        <c:crossAx val="122052608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1140,7 +1134,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60417152"/>
+        <c:axId val="122052608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1170,7 +1164,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96385536"/>
+        <c:crossAx val="122310656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1577,11 +1571,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="98734080"/>
-        <c:axId val="60419456"/>
+        <c:axId val="122311680"/>
+        <c:axId val="122054912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98734080"/>
+        <c:axId val="122311680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1601,7 +1595,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60419456"/>
+        <c:crossAx val="122054912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1609,7 +1603,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60419456"/>
+        <c:axId val="122054912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1639,7 +1633,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98734080"/>
+        <c:crossAx val="122311680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1839,11 +1833,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="98734592"/>
-        <c:axId val="60421760"/>
+        <c:axId val="122312192"/>
+        <c:axId val="122057216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98734592"/>
+        <c:axId val="122312192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1863,7 +1857,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60421760"/>
+        <c:crossAx val="122057216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1871,7 +1865,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60421760"/>
+        <c:axId val="122057216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1901,7 +1895,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98734592"/>
+        <c:crossAx val="122312192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2101,11 +2095,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="98735104"/>
-        <c:axId val="98811904"/>
+        <c:axId val="122312704"/>
+        <c:axId val="122059520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98735104"/>
+        <c:axId val="122312704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2125,7 +2119,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98811904"/>
+        <c:crossAx val="122059520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2133,7 +2127,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98811904"/>
+        <c:axId val="122059520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2163,7 +2157,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98735104"/>
+        <c:crossAx val="122312704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2347,11 +2341,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96384512"/>
-        <c:axId val="98814208"/>
+        <c:axId val="97438720"/>
+        <c:axId val="122815616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96384512"/>
+        <c:axId val="97438720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2371,7 +2365,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98814208"/>
+        <c:crossAx val="122815616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2379,7 +2373,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98814208"/>
+        <c:axId val="122815616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2409,7 +2403,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96384512"/>
+        <c:crossAx val="97438720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2913,8 +2907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="BB24" sqref="BB24"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2979,16 +2973,16 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -3006,16 +3000,16 @@
         <v>5</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
@@ -3033,16 +3027,16 @@
         <v>5</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="AA1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:57" x14ac:dyDescent="0.25">
@@ -3144,16 +3138,16 @@
         <v>5</v>
       </c>
       <c r="AH2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AI2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="AK2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AL2" s="1" t="s">
         <v>2</v>
@@ -3171,16 +3165,16 @@
         <v>5</v>
       </c>
       <c r="AQ2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AS2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AR2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="AT2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AU2" s="1" t="s">
         <v>2</v>
@@ -3198,16 +3192,16 @@
         <v>5</v>
       </c>
       <c r="AZ2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BB2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="BA2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="BB2" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="BC2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:57" x14ac:dyDescent="0.25">
@@ -5945,142 +5939,65 @@
       </c>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="A48" s="6"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
-      <c r="F48" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
       <c r="H48" s="7"/>
     </row>
     <row r="49" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H49" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="1"/>
     </row>
     <row r="50" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A50" s="7">
-        <v>5000</v>
-      </c>
-      <c r="B50" s="7">
-        <v>5000</v>
-      </c>
-      <c r="C50" s="7">
-        <v>51133499.100000001</v>
-      </c>
-      <c r="D50" s="7">
-        <v>570312074.70000005</v>
-      </c>
-      <c r="E50" s="7">
-        <v>349233080.30000001</v>
-      </c>
-      <c r="F50" s="7">
-        <v>58074828.799999997</v>
-      </c>
-      <c r="G50" s="7">
-        <v>758622719.79999995</v>
-      </c>
-      <c r="H50" s="7">
-        <v>0</v>
-      </c>
-      <c r="I50">
-        <v>321370075.30000001</v>
-      </c>
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
     </row>
     <row r="51" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A51" s="7">
-        <v>5000</v>
-      </c>
-      <c r="B51" s="7">
-        <v>10000</v>
-      </c>
-      <c r="C51" s="7">
-        <v>104076700.8</v>
-      </c>
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
       <c r="D51" s="7"/>
-      <c r="E51" s="7">
-        <v>696298163.29999995</v>
-      </c>
-      <c r="F51" s="7">
-        <v>115396988.59999999</v>
-      </c>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
       <c r="G51" s="7"/>
-      <c r="H51" s="7">
-        <v>0</v>
-      </c>
+      <c r="H51" s="7"/>
     </row>
     <row r="52" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A52" s="7">
-        <v>5000</v>
-      </c>
-      <c r="B52" s="7">
-        <v>50000</v>
-      </c>
-      <c r="C52" s="7">
-        <v>513527384</v>
-      </c>
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
       <c r="D52" s="7"/>
-      <c r="E52" s="7">
-        <v>3502460776.4000001</v>
-      </c>
-      <c r="F52" s="7">
-        <v>577250410.70000005</v>
-      </c>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
       <c r="G52" s="7"/>
-      <c r="H52" s="7">
-        <v>0</v>
-      </c>
+      <c r="H52" s="7"/>
     </row>
     <row r="53" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A53" s="7">
-        <v>5000</v>
-      </c>
-      <c r="B53" s="7">
-        <v>100000</v>
-      </c>
-      <c r="C53" s="7">
-        <v>1033611071.6</v>
-      </c>
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
-      <c r="F53" s="7">
-        <v>1159647485.2</v>
-      </c>
+      <c r="F53" s="7"/>
       <c r="G53" s="7"/>
-      <c r="H53" s="7">
-        <v>0</v>
-      </c>
+      <c r="H53" s="7"/>
     </row>
     <row r="54" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
@@ -6088,136 +6005,61 @@
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
-      <c r="F54" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
       <c r="H54" s="7"/>
     </row>
     <row r="55" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H55" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A55" s="7"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="1"/>
     </row>
     <row r="56" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A56" s="7">
-        <v>10000</v>
-      </c>
-      <c r="B56" s="7">
-        <v>5000</v>
-      </c>
-      <c r="C56" s="7">
-        <v>53262135.600000001</v>
-      </c>
-      <c r="D56" s="7">
-        <v>570063835.70000005</v>
-      </c>
-      <c r="E56" s="7">
-        <v>649312973.5</v>
-      </c>
-      <c r="F56" s="7">
-        <v>59370671.899999999</v>
-      </c>
-      <c r="G56" s="7">
-        <v>758356146.70000005</v>
-      </c>
-      <c r="H56" s="7">
-        <v>0</v>
-      </c>
-      <c r="I56">
-        <v>455708963.5</v>
-      </c>
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
     </row>
     <row r="57" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A57" s="7">
-        <v>10000</v>
-      </c>
-      <c r="B57" s="7">
-        <v>10000</v>
-      </c>
-      <c r="C57" s="7">
-        <v>106518125.3</v>
-      </c>
+      <c r="A57" s="7"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
       <c r="D57" s="7"/>
-      <c r="E57" s="7">
-        <v>1307197254.8</v>
-      </c>
-      <c r="F57" s="7">
-        <v>116606223.7</v>
-      </c>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
       <c r="G57" s="7"/>
-      <c r="H57" s="7">
-        <v>0</v>
-      </c>
+      <c r="H57" s="7"/>
       <c r="AH57" s="2"/>
     </row>
     <row r="58" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A58" s="7">
-        <v>10000</v>
-      </c>
-      <c r="B58" s="7">
-        <v>50000</v>
-      </c>
-      <c r="C58" s="7">
-        <v>522000929.69999999</v>
-      </c>
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
       <c r="D58" s="7"/>
-      <c r="E58" s="7">
-        <v>6546358859</v>
-      </c>
-      <c r="F58" s="7">
-        <v>581778089.10000002</v>
-      </c>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
       <c r="G58" s="7"/>
-      <c r="H58" s="7">
-        <v>0</v>
-      </c>
+      <c r="H58" s="7"/>
     </row>
     <row r="59" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A59" s="7">
-        <v>10000</v>
-      </c>
-      <c r="B59" s="7">
-        <v>100000</v>
-      </c>
-      <c r="C59" s="7">
-        <v>1093636158.4000001</v>
-      </c>
+      <c r="A59" s="7"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
-      <c r="F59" s="7">
-        <v>1165158093.2</v>
-      </c>
+      <c r="F59" s="7"/>
       <c r="G59" s="7"/>
-      <c r="H59" s="7">
-        <v>0</v>
-      </c>
+      <c r="H59" s="7"/>
     </row>
     <row r="60" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
@@ -6230,124 +6072,53 @@
       <c r="H60" s="7"/>
     </row>
     <row r="61" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G61" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H61" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A61" s="7"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+      <c r="I61" s="1"/>
     </row>
     <row r="62" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A62" s="7">
-        <v>50000</v>
-      </c>
-      <c r="B62" s="7">
-        <v>5000</v>
-      </c>
-      <c r="C62" s="7">
-        <v>60102177.5</v>
-      </c>
-      <c r="D62" s="7">
-        <v>567922284.5</v>
-      </c>
-      <c r="E62">
-        <v>9054742719</v>
-      </c>
-      <c r="F62" s="7">
-        <v>65438086.299999997</v>
-      </c>
-      <c r="G62" s="7">
-        <v>759719747</v>
-      </c>
-      <c r="H62" s="7">
-        <v>0</v>
-      </c>
-      <c r="I62">
-        <v>1770603799.3333333</v>
-      </c>
+      <c r="A62" s="7"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
     </row>
     <row r="63" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A63" s="7">
-        <v>50000</v>
-      </c>
-      <c r="B63" s="7">
-        <v>10000</v>
-      </c>
-      <c r="C63" s="7">
-        <v>118687686.90000001</v>
-      </c>
+      <c r="A63" s="7"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
       <c r="D63" s="7"/>
-      <c r="E63">
-        <v>18126616842.099998</v>
-      </c>
-      <c r="F63" s="7">
-        <v>131681648.09999999</v>
-      </c>
+      <c r="F63" s="7"/>
       <c r="G63" s="7"/>
-      <c r="H63" s="7">
-        <v>0</v>
-      </c>
+      <c r="H63" s="7"/>
     </row>
     <row r="64" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A64" s="7">
-        <v>50000</v>
-      </c>
-      <c r="B64" s="7">
-        <v>50000</v>
-      </c>
-      <c r="C64" s="7">
-        <v>590382890</v>
-      </c>
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
-      <c r="F64" s="7">
-        <v>651354330.70000005</v>
-      </c>
+      <c r="F64" s="7"/>
       <c r="G64" s="7"/>
-      <c r="H64" s="7">
-        <v>0</v>
-      </c>
+      <c r="H64" s="7"/>
     </row>
     <row r="65" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A65" s="7">
-        <v>50000</v>
-      </c>
-      <c r="B65" s="7">
-        <v>100000</v>
-      </c>
-      <c r="C65" s="7">
-        <v>1181887848.0999999</v>
-      </c>
+      <c r="A65" s="7"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
-      <c r="F65" s="7">
-        <v>1296009590.5999999</v>
-      </c>
+      <c r="F65" s="7"/>
       <c r="G65" s="7"/>
-      <c r="H65" s="7">
-        <v>0</v>
-      </c>
+      <c r="H65" s="7"/>
     </row>
     <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
@@ -6360,19 +6131,13 @@
       <c r="H66" s="7"/>
     </row>
     <row r="67" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
-        <v>7</v>
-      </c>
+      <c r="A67" s="6"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
-      <c r="F67" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G67" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
       <c r="H67" s="7"/>
       <c r="I67" s="1"/>
       <c r="W67" t="s">
@@ -6380,159 +6145,62 @@
       </c>
     </row>
     <row r="68" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F68" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G68" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H68" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A68" s="7"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+      <c r="I68" s="1"/>
     </row>
     <row r="69" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A69" s="7">
-        <v>5000</v>
-      </c>
-      <c r="B69" s="7">
-        <v>5000</v>
-      </c>
-      <c r="C69" s="7">
-        <f t="shared" ref="C69:I69" si="3">C50*10</f>
-        <v>511334991</v>
-      </c>
-      <c r="D69" s="7">
-        <f t="shared" si="3"/>
-        <v>5703120747</v>
-      </c>
-      <c r="E69" s="7">
-        <f t="shared" si="3"/>
-        <v>3492330803</v>
-      </c>
-      <c r="F69" s="7">
-        <f t="shared" si="3"/>
-        <v>580748288</v>
-      </c>
-      <c r="G69" s="7">
-        <f t="shared" si="3"/>
-        <v>7586227198</v>
-      </c>
-      <c r="H69" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I69" s="7">
-        <f t="shared" si="3"/>
-        <v>3213700753</v>
-      </c>
+      <c r="A69" s="7"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
+      <c r="I69" s="7"/>
       <c r="W69" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A70" s="7">
-        <v>5000</v>
-      </c>
-      <c r="B70" s="7">
-        <v>10000</v>
-      </c>
-      <c r="C70" s="7">
-        <f t="shared" ref="C70:H70" si="4">C51*10</f>
-        <v>1040767008</v>
-      </c>
+      <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
       <c r="D70" s="7"/>
-      <c r="E70" s="7">
-        <f t="shared" si="4"/>
-        <v>6962981633</v>
-      </c>
-      <c r="F70" s="7">
-        <f t="shared" si="4"/>
-        <v>1153969886</v>
-      </c>
-      <c r="G70" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H70" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
     </row>
     <row r="71" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A71" s="7">
-        <v>5000</v>
-      </c>
-      <c r="B71" s="7">
-        <v>50000</v>
-      </c>
-      <c r="C71" s="7">
-        <f t="shared" ref="C71:H71" si="5">C52*10</f>
-        <v>5135273840</v>
-      </c>
+      <c r="A71" s="7"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
       <c r="D71" s="7"/>
-      <c r="E71" s="7">
-        <f t="shared" si="5"/>
-        <v>35024607764</v>
-      </c>
-      <c r="F71" s="7">
-        <f t="shared" si="5"/>
-        <v>5772504107</v>
-      </c>
-      <c r="G71" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H71" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
       <c r="W71" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A72" s="7">
-        <v>5000</v>
-      </c>
-      <c r="B72" s="7">
-        <v>100000</v>
-      </c>
-      <c r="C72" s="7">
-        <f t="shared" ref="C72:H72" si="6">C53*10</f>
-        <v>10336110716</v>
-      </c>
+      <c r="A72" s="7"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
-      <c r="F72" s="7">
-        <f t="shared" si="6"/>
-        <v>11596474852</v>
-      </c>
-      <c r="G72" s="7">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H72" s="7">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
     </row>
     <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
@@ -6540,168 +6208,67 @@
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
       <c r="E73" s="7"/>
-      <c r="F73" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G73" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
       <c r="H73" s="7"/>
       <c r="W73" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E74" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F74" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G74" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H74" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A74" s="7"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
+      <c r="I74" s="1"/>
     </row>
     <row r="75" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A75" s="7">
-        <v>10000</v>
-      </c>
-      <c r="B75" s="7">
-        <v>5000</v>
-      </c>
-      <c r="C75" s="7">
-        <f t="shared" ref="C75:I75" si="7">C56*10</f>
-        <v>532621356</v>
-      </c>
-      <c r="D75" s="7">
-        <f t="shared" si="7"/>
-        <v>5700638357</v>
-      </c>
-      <c r="E75" s="7">
-        <f t="shared" si="7"/>
-        <v>6493129735</v>
-      </c>
-      <c r="F75" s="7">
-        <f t="shared" si="7"/>
-        <v>593706719</v>
-      </c>
-      <c r="G75" s="7">
-        <f t="shared" si="7"/>
-        <v>7583561467</v>
-      </c>
-      <c r="H75" s="7">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I75" s="7">
-        <f t="shared" si="7"/>
-        <v>4557089635</v>
-      </c>
+      <c r="A75" s="7"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
+      <c r="I75" s="7"/>
       <c r="W75" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A76" s="7">
-        <v>10000</v>
-      </c>
-      <c r="B76" s="7">
-        <v>10000</v>
-      </c>
-      <c r="C76" s="7">
-        <f t="shared" ref="C76:H76" si="8">C57*10</f>
-        <v>1065181253</v>
-      </c>
+      <c r="A76" s="7"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
       <c r="D76" s="7"/>
-      <c r="E76" s="7">
-        <f t="shared" si="8"/>
-        <v>13071972548</v>
-      </c>
-      <c r="F76" s="7">
-        <f t="shared" si="8"/>
-        <v>1166062237</v>
-      </c>
-      <c r="G76" s="7">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H76" s="7">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
     </row>
     <row r="77" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A77" s="7">
-        <v>10000</v>
-      </c>
-      <c r="B77" s="7">
-        <v>50000</v>
-      </c>
-      <c r="C77" s="7">
-        <f t="shared" ref="C77:H77" si="9">C58*10</f>
-        <v>5220009297</v>
-      </c>
+      <c r="A77" s="7"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
       <c r="D77" s="7"/>
-      <c r="E77" s="7">
-        <f t="shared" si="9"/>
-        <v>65463588590</v>
-      </c>
-      <c r="F77" s="7">
-        <f t="shared" si="9"/>
-        <v>5817780891</v>
-      </c>
-      <c r="G77" s="7">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="H77" s="7">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
     </row>
     <row r="78" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A78" s="7">
-        <v>10000</v>
-      </c>
-      <c r="B78" s="7">
-        <v>100000</v>
-      </c>
-      <c r="C78" s="7">
-        <f t="shared" ref="C78:H78" si="10">C59*10</f>
-        <v>10936361584</v>
-      </c>
+      <c r="A78" s="7"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
       <c r="D78" s="7"/>
       <c r="E78" s="7"/>
-      <c r="F78" s="7">
-        <f t="shared" si="10"/>
-        <v>11651580932</v>
-      </c>
-      <c r="G78" s="7">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="H78" s="7">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
     </row>
     <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
@@ -6720,154 +6287,60 @@
       <c r="AA79" s="1"/>
     </row>
     <row r="80" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A80" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E80" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G80" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H80" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I80" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A80" s="7"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="7"/>
+      <c r="I80" s="1"/>
       <c r="K80" s="3"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="7">
-        <v>50000</v>
-      </c>
-      <c r="B81" s="7">
-        <v>5000</v>
-      </c>
-      <c r="C81" s="7">
-        <f t="shared" ref="C81:I81" si="11">C62*10</f>
-        <v>601021775</v>
-      </c>
-      <c r="D81" s="7">
-        <f t="shared" si="11"/>
-        <v>5679222845</v>
-      </c>
-      <c r="E81" s="7">
-        <f t="shared" si="11"/>
-        <v>90547427190</v>
-      </c>
-      <c r="F81" s="7">
-        <f t="shared" si="11"/>
-        <v>654380863</v>
-      </c>
-      <c r="G81" s="7">
-        <f t="shared" si="11"/>
-        <v>7597197470</v>
-      </c>
-      <c r="H81" s="7">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="I81" s="7">
-        <f t="shared" si="11"/>
-        <v>17706037993.333332</v>
-      </c>
+      <c r="A81" s="7"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
+      <c r="I81" s="7"/>
       <c r="K81" s="3"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" s="7">
-        <v>50000</v>
-      </c>
-      <c r="B82" s="7">
-        <v>10000</v>
-      </c>
-      <c r="C82" s="7">
-        <f t="shared" ref="C82:H82" si="12">C63*10</f>
-        <v>1186876869</v>
-      </c>
+      <c r="A82" s="7"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="7"/>
       <c r="D82" s="7"/>
-      <c r="E82" s="7">
-        <f t="shared" si="12"/>
-        <v>181266168421</v>
-      </c>
-      <c r="F82" s="7">
-        <f t="shared" si="12"/>
-        <v>1316816481</v>
-      </c>
-      <c r="G82" s="7">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="H82" s="7">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
+      <c r="H82" s="7"/>
       <c r="K82" s="3"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="7">
-        <v>50000</v>
-      </c>
-      <c r="B83" s="7">
-        <v>50000</v>
-      </c>
-      <c r="C83" s="7">
-        <f t="shared" ref="C83:H83" si="13">C64*10</f>
-        <v>5903828900</v>
-      </c>
+      <c r="A83" s="7"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="7"/>
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
-      <c r="F83" s="7">
-        <f t="shared" si="13"/>
-        <v>6513543307</v>
-      </c>
-      <c r="G83" s="7">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="H83" s="7">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="7"/>
       <c r="K83" s="3"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="7">
-        <v>50000</v>
-      </c>
-      <c r="B84" s="7">
-        <v>100000</v>
-      </c>
-      <c r="C84" s="7">
-        <f t="shared" ref="C84:H84" si="14">C65*10</f>
-        <v>11818878481</v>
-      </c>
+      <c r="A84" s="7"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
       <c r="D84" s="7"/>
       <c r="E84" s="7"/>
-      <c r="F84" s="7">
-        <f t="shared" si="14"/>
-        <v>12960095906</v>
-      </c>
-      <c r="G84" s="7">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="H84" s="7">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="7"/>
       <c r="K84" s="3"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>